<commit_message>
Modelo Físico incrementado, a terminar.
</commit_message>
<xml_diff>
--- a/Banco de Dados/Modelagem/Esboço Modelo Físico.xlsx
+++ b/Banco de Dados/Modelagem/Esboço Modelo Físico.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20376"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fic\Desktop\Projeto_HROADS_SENAI\Banco de Dados\Modelagem\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E1DB1BF-CEFD-41EE-9573-395B7801170E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="75" windowWidth="27795" windowHeight="8265"/>
+    <workbookView xWindow="360" yWindow="72" windowWidth="27792" windowHeight="8268" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
   <si>
     <t>Nome</t>
   </si>
@@ -100,14 +106,40 @@
   </si>
   <si>
     <t>Regen</t>
+  </si>
+  <si>
+    <t>nomeTipoHabi</t>
+  </si>
+  <si>
+    <t>values</t>
+  </si>
+  <si>
+    <t>classe</t>
+  </si>
+  <si>
+    <t>classe x habilidades</t>
+  </si>
+  <si>
+    <t>idClasseHabi</t>
+  </si>
+  <si>
+    <t>Cetro King</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -123,7 +155,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -212,34 +244,26 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -247,10 +271,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -261,6 +297,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -268,7 +307,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -306,9 +345,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -341,9 +380,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -376,9 +432,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -551,312 +624,408 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="2" t="s">
+    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H1" s="15"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="3"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="14"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
-      <c r="M2" s="3"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="6"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="6"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="M2" s="2"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="3"/>
+      <c r="I3" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="I4" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="J4" s="10" t="s">
+      <c r="J4" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="6"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="5" t="s">
+      <c r="K4" s="10"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" s="1"/>
+      <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="4"/>
-      <c r="J5" s="10" t="s">
+      <c r="I5" s="10">
+        <v>1</v>
+      </c>
+      <c r="J5" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="6"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="5" t="s">
+      <c r="K5" s="10"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
+      <c r="B6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="6"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="10" t="s">
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="3"/>
+      <c r="I6" s="10">
+        <v>2</v>
+      </c>
+      <c r="J6" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="6"/>
-    </row>
-    <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="7"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="9"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="8" t="s">
+      <c r="K6" s="10"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+    </row>
+    <row r="7" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="4"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="6"/>
+      <c r="I7" s="10">
+        <v>3</v>
+      </c>
+      <c r="J7" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="9"/>
-    </row>
-    <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="2" t="s">
-        <v>16</v>
-      </c>
+      <c r="K7" s="10"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+    </row>
+    <row r="8" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="5"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2" t="s">
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H9" s="2"/>
+      <c r="J9" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="M9" s="2"/>
-      <c r="N9" s="3"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="6"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="K9" s="12"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="12"/>
+      <c r="N9" s="14"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="3"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L11" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="M11" s="2"/>
+      <c r="N11" s="3"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="2">
+        <v>1</v>
+      </c>
+      <c r="G12" s="2">
+        <v>1</v>
+      </c>
+      <c r="H12" s="2">
+        <v>1</v>
+      </c>
+      <c r="J12" s="1">
+        <v>1</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L12" s="2">
+        <v>1</v>
+      </c>
+      <c r="M12" s="2"/>
+      <c r="N12" s="3"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2">
+        <v>2</v>
+      </c>
+      <c r="G13" s="2">
+        <v>2</v>
+      </c>
+      <c r="H13" s="2">
+        <v>1</v>
+      </c>
+      <c r="J13" s="1">
+        <v>2</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L13" s="2">
+        <v>2</v>
+      </c>
+      <c r="M13" s="2"/>
+      <c r="N13" s="3"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2">
+        <v>3</v>
+      </c>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="J14" s="1">
+        <v>3</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L14" s="2">
+        <v>3</v>
+      </c>
+      <c r="M14" s="2"/>
+      <c r="N14" s="3"/>
+    </row>
+    <row r="15" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F15" s="7">
+        <v>4</v>
+      </c>
+      <c r="J15" s="4">
+        <v>4</v>
+      </c>
+      <c r="K15" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="L15" s="5">
+        <v>4</v>
+      </c>
+      <c r="M15" s="5"/>
+      <c r="N15" s="6"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="12"/>
+      <c r="C16" s="14"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B17" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" s="7"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>1</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C18" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>2</v>
+      </c>
+      <c r="B19" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="C19" s="3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>3</v>
+      </c>
+      <c r="B20" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="C20" s="3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="4">
+        <v>4</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F11" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="J11" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="K11" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="6"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
-        <v>1</v>
-      </c>
-      <c r="B12" s="5">
-        <v>40</v>
-      </c>
-      <c r="C12" s="5">
-        <v>25</v>
-      </c>
-      <c r="D12" s="5">
-        <v>30</v>
-      </c>
-      <c r="E12" s="13">
+      <c r="C21" s="6">
         <v>50</v>
       </c>
-      <c r="F12" s="5">
-        <v>1</v>
-      </c>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="J12" s="4">
-        <v>1</v>
-      </c>
-      <c r="K12" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="6"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="5">
-        <v>2</v>
-      </c>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="J13" s="4">
-        <v>2</v>
-      </c>
-      <c r="K13" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="L13" s="5"/>
-      <c r="M13" s="5"/>
-      <c r="N13" s="6"/>
-    </row>
-    <row r="14" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="7"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="J14" s="7">
-        <v>3</v>
-      </c>
-      <c r="K14" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="L14" s="8"/>
-      <c r="M14" s="8"/>
-      <c r="N14" s="9"/>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="J9:N9"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>